<commit_message>
update to add data to neo4j
</commit_message>
<xml_diff>
--- a/Neo4j/BulkChem/pka/sorting_data.xlsx
+++ b/Neo4j/BulkChem/pka/sorting_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\McQuade-Chem-ML\Neo4j\BulkChem\pka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4FCDE8-D9E7-460F-AB26-7028AAABD5BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A0AFD-DEF5-4476-B218-C3C44B5AF8F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>Conjugate Acid</t>
   </si>
@@ -99,9 +99,6 @@
     <t>ON(*)*</t>
   </si>
   <si>
-    <t>ON</t>
-  </si>
-  <si>
     <t>OP([O-])([O-])=O</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>5.2</t>
   </si>
   <si>
-    <t>5.96</t>
-  </si>
-  <si>
     <t>12.50</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
   </si>
   <si>
     <t>[O-]N(*)*</t>
-  </si>
-  <si>
-    <t>[O-]N</t>
   </si>
   <si>
     <t>[O-]P([O-])([O-])=O</t>
@@ -723,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,10 +743,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -763,10 +754,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -774,10 +765,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -785,7 +776,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -793,10 +784,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -804,10 +795,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -815,10 +806,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -826,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -837,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -859,7 +850,7 @@
         <v>11.1</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -867,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -875,7 +866,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -883,18 +874,18 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -902,10 +893,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -913,10 +904,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -924,10 +915,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -935,10 +926,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -946,10 +937,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -957,10 +948,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -968,10 +959,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -979,10 +970,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -990,10 +981,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1001,10 +992,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1012,10 +1003,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1023,10 +1014,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1034,10 +1025,10 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1045,10 +1036,10 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1056,10 +1047,10 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1067,10 +1058,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1078,10 +1069,10 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1089,21 +1080,10 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>